<commit_message>
Se ha realizado el programa de modificar usuarios y equipos, también se finaliza asesorias
</commit_message>
<xml_diff>
--- a/usuarios_subida.xlsx
+++ b/usuarios_subida.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{05728588-28D6-4772-9919-5336BC9C9C5C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{54C4399F-70BC-47D8-A0D4-D9541F6CFE13}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estudiantes" sheetId="1" r:id="rId1"/>
@@ -449,12 +449,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="4" max="4" width="23.77734375" customWidth="1"/>
     <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -523,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C2C07A-5620-4A67-B0DC-0BD246A1EDB9}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,7 +708,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>